<commit_message>
ganti cell H ke F
</commit_message>
<xml_diff>
--- a/public/write.xlsx
+++ b/public/write.xlsx
@@ -35,58 +35,58 @@
     <t>Keterangan</t>
   </si>
   <si>
-    <t>Imam Satya Wedhatama</t>
-  </si>
-  <si>
-    <t>6:40</t>
-  </si>
-  <si>
-    <t>19:32</t>
-  </si>
-  <si>
-    <t>Bahtiar</t>
-  </si>
-  <si>
-    <t>6:41</t>
-  </si>
-  <si>
-    <t>16:05</t>
-  </si>
-  <si>
-    <t>Ananto</t>
-  </si>
-  <si>
-    <t>6:54</t>
-  </si>
-  <si>
-    <t>Hudi Javariawan</t>
-  </si>
-  <si>
-    <t>7:09</t>
-  </si>
-  <si>
-    <t>Sri Astuti - 340055436</t>
-  </si>
-  <si>
-    <t>16:07</t>
-  </si>
-  <si>
-    <t>7:13</t>
-  </si>
-  <si>
-    <t>Dedi Saputra - 340017865</t>
-  </si>
-  <si>
-    <t>7:34</t>
-  </si>
-  <si>
-    <t>17:00</t>
-  </si>
-  <si>
-    <t>Ananto Yanuar</t>
-  </si>
-  <si>
-    <t>16:41</t>
+    <t>Yudha Subakti - 340059291</t>
+  </si>
+  <si>
+    <t>7:02</t>
+  </si>
+  <si>
+    <t>18:20</t>
+  </si>
+  <si>
+    <t>Irwan Kurniawan-340016236</t>
+  </si>
+  <si>
+    <t>7:05</t>
+  </si>
+  <si>
+    <t>16:52</t>
+  </si>
+  <si>
+    <t>Agus Santoso</t>
+  </si>
+  <si>
+    <t>7:06</t>
+  </si>
+  <si>
+    <t>16:54</t>
+  </si>
+  <si>
+    <t>MAYA NOVITA SARI - 58827</t>
+  </si>
+  <si>
+    <t>7:14</t>
+  </si>
+  <si>
+    <t>18:16</t>
+  </si>
+  <si>
+    <t>Reny Anggraeni - 34005929</t>
+  </si>
+  <si>
+    <t>7:17</t>
+  </si>
+  <si>
+    <t>18:02</t>
+  </si>
+  <si>
+    <t>Sri Pura - 3400013224</t>
+  </si>
+  <si>
+    <t>7:33</t>
+  </si>
+  <si>
+    <t>16:17</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="I4" sqref="I4"/>
@@ -590,7 +590,9 @@
       <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="5"/>
@@ -601,12 +603,14 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="3"/>
+        <v>16</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="5"/>
@@ -617,13 +621,13 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="4"/>
@@ -635,13 +639,13 @@
         <v>6</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="E9" s="4"/>
       <c r="F9" s="4"/>
@@ -649,15 +653,9 @@
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="2">
-        <v>7</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
       <c r="D10" s="3"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
@@ -674,23 +672,13 @@
       <c r="G11" s="5"/>
       <c r="H11" s="6"/>
     </row>
-    <row r="12" spans="1:10">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
-    </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>

</xml_diff>